<commit_message>
07. Mengisi Resep Pasien
DO:
- Mengisi database tabel obat, penyakit, dan tindakan
- Menambahkan fungsi untuk dokter meng-inputkan resep pasien (dengan
banyak fungsi-fungsi penunjang lainnya)
- Revisi fungsi autonumber di service server administrator sesuai kode
yg disepakati

OBSTACLES:
- crashed of commit so the file were merged forcely (BagPendaftaran) and
they don't fix it as soon as possible

TO DO:
- Mengisi database tabel master layanan lab dan layanan kecantikan
- Merevisi input resep pasien
</commit_message>
<xml_diff>
--- a/Project/Database/penyakit_anak.xlsx
+++ b/Project/Database/penyakit_anak.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\S1 Sistem Informasi 2012\Semester 6\Pengembangan Sistem Informasi\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Kulit kuning, demam</t>
   </si>
@@ -194,25 +189,103 @@
     <t>Batuk rejan</t>
   </si>
   <si>
-    <t>demam dan ruam yang menyebar  ke seluruh tubuh</t>
-  </si>
-  <si>
-    <t>Rubella(campak)</t>
-  </si>
-  <si>
-    <t>gejala</t>
-  </si>
-  <si>
-    <t>penyakit</t>
-  </si>
-  <si>
-    <t>id_penyakit</t>
+    <t>Rubella (campak)</t>
+  </si>
+  <si>
+    <t>Demam dan ruam yang menyebar ke seluruh tubuh</t>
+  </si>
+  <si>
+    <t>P0001</t>
+  </si>
+  <si>
+    <t>P0002</t>
+  </si>
+  <si>
+    <t>P0003</t>
+  </si>
+  <si>
+    <t>P0004</t>
+  </si>
+  <si>
+    <t>P0005</t>
+  </si>
+  <si>
+    <t>P0006</t>
+  </si>
+  <si>
+    <t>P0007</t>
+  </si>
+  <si>
+    <t>P0008</t>
+  </si>
+  <si>
+    <t>P0009</t>
+  </si>
+  <si>
+    <t>P0010</t>
+  </si>
+  <si>
+    <t>P0011</t>
+  </si>
+  <si>
+    <t>P0012</t>
+  </si>
+  <si>
+    <t>P0013</t>
+  </si>
+  <si>
+    <t>P0014</t>
+  </si>
+  <si>
+    <t>P0015</t>
+  </si>
+  <si>
+    <t>P0016</t>
+  </si>
+  <si>
+    <t>P0017</t>
+  </si>
+  <si>
+    <t>P0018</t>
+  </si>
+  <si>
+    <t>P0019</t>
+  </si>
+  <si>
+    <t>P0020</t>
+  </si>
+  <si>
+    <t>P0021</t>
+  </si>
+  <si>
+    <t>P0022</t>
+  </si>
+  <si>
+    <t>P0023</t>
+  </si>
+  <si>
+    <t>P0024</t>
+  </si>
+  <si>
+    <t>P0025</t>
+  </si>
+  <si>
+    <t>P0026</t>
+  </si>
+  <si>
+    <t>P0027</t>
+  </si>
+  <si>
+    <t>P0028</t>
+  </si>
+  <si>
+    <t>P0029</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -305,7 +378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,7 +413,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,262 +590,341 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>76</v>
+      </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>84</v>
+      </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>